<commit_message>
update example7 with vmx 23.2
</commit_message>
<xml_diff>
--- a/lab1_byot/examples/example7.xlsx
+++ b/lab1_byot/examples/example7.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11116"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Gilbertor/PycharmProjects/vjunos_kvm/lab1_byot/examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BDCE35F-1B6B-A843-83AE-6275029C3B26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42630E28-23B1-A94B-9B33-16A9A177F5EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="35380" yWindow="3640" windowWidth="32880" windowHeight="19760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="35380" yWindow="1840" windowWidth="32880" windowHeight="19760" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SRX" sheetId="1" r:id="rId1"/>
@@ -199,9 +199,6 @@
     <t>vmx-vcp</t>
   </si>
   <si>
-    <t>22.4R2.8</t>
-  </si>
-  <si>
     <t>vmx-vfp</t>
   </si>
   <si>
@@ -224,6 +221,9 @@
   </si>
   <si>
     <t>lab1_vfp0_r4</t>
+  </si>
+  <si>
+    <t>23.2R2-S1.3</t>
   </si>
 </sst>
 </file>
@@ -405,9 +405,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -445,7 +445,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -551,7 +551,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -693,7 +693,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -703,7 +703,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
@@ -989,15 +989,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92CF0E90-D97A-EC44-A339-6A36611C0CEE}">
   <dimension ref="A1:Q31"/>
   <sheetViews>
-    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24:Q24"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="5.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="4.5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.33203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14.6640625" bestFit="1" customWidth="1"/>
@@ -1090,7 +1090,7 @@
         <v>56</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>57</v>
+        <v>65</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>41</v>
@@ -1120,16 +1120,16 @@
         <v>0</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>57</v>
+        <v>65</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>41</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="4"/>
@@ -1152,7 +1152,7 @@
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A5" s="13" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B5" s="13"/>
       <c r="C5" s="13"/>
@@ -1179,13 +1179,13 @@
         <v>56</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>57</v>
+        <v>65</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>41</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>43</v>
@@ -1209,16 +1209,16 @@
         <v>0</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>57</v>
+        <v>65</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>41</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
@@ -1239,7 +1239,7 @@
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A8" s="16" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B8" s="16"/>
       <c r="C8" s="16"/>
@@ -1266,13 +1266,13 @@
         <v>56</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>57</v>
+        <v>65</v>
       </c>
       <c r="D9" s="3" t="s">
         <v>41</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F9" s="3" t="s">
         <v>44</v>
@@ -1296,16 +1296,16 @@
         <v>0</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>57</v>
+        <v>65</v>
       </c>
       <c r="D10" s="3" t="s">
         <v>41</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F10" s="4"/>
       <c r="G10" s="4"/>
@@ -1326,7 +1326,7 @@
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A11" s="13" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B11" s="13"/>
       <c r="C11" s="13"/>
@@ -1353,13 +1353,13 @@
         <v>56</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>57</v>
+        <v>65</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>41</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F12" s="1" t="s">
         <v>45</v>
@@ -1383,16 +1383,16 @@
         <v>0</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>57</v>
+        <v>65</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>41</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
@@ -2433,12 +2433,6 @@
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="A12:Q12"/>
-    <mergeCell ref="A2:Q2"/>
-    <mergeCell ref="A4:Q4"/>
-    <mergeCell ref="A6:Q6"/>
-    <mergeCell ref="A8:Q8"/>
-    <mergeCell ref="A10:Q10"/>
     <mergeCell ref="A26:Q26"/>
     <mergeCell ref="A28:Q28"/>
     <mergeCell ref="A14:Q14"/>
@@ -2447,6 +2441,12 @@
     <mergeCell ref="A20:Q20"/>
     <mergeCell ref="A22:Q22"/>
     <mergeCell ref="A24:Q24"/>
+    <mergeCell ref="A12:Q12"/>
+    <mergeCell ref="A2:Q2"/>
+    <mergeCell ref="A4:Q4"/>
+    <mergeCell ref="A6:Q6"/>
+    <mergeCell ref="A8:Q8"/>
+    <mergeCell ref="A10:Q10"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3793,13 +3793,6 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="A30:T30"/>
-    <mergeCell ref="A20:T20"/>
-    <mergeCell ref="A24:T24"/>
-    <mergeCell ref="A32:T32"/>
-    <mergeCell ref="A8:T8"/>
-    <mergeCell ref="A22:T22"/>
-    <mergeCell ref="A12:T12"/>
     <mergeCell ref="A2:T2"/>
     <mergeCell ref="A16:T16"/>
     <mergeCell ref="A10:T10"/>
@@ -3809,6 +3802,13 @@
     <mergeCell ref="A18:T18"/>
     <mergeCell ref="A26:T26"/>
     <mergeCell ref="A6:T6"/>
+    <mergeCell ref="A30:T30"/>
+    <mergeCell ref="A20:T20"/>
+    <mergeCell ref="A24:T24"/>
+    <mergeCell ref="A32:T32"/>
+    <mergeCell ref="A8:T8"/>
+    <mergeCell ref="A22:T22"/>
+    <mergeCell ref="A12:T12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>